<commit_message>
Umstrukturierung und Excel Rauschmessung + Python auswertung angefangen
</commit_message>
<xml_diff>
--- a/PhasenMethode/Messungen+Auswertung/Messungen/1312_HO_Amplitudenuntersuchung/05_InterleavingCodeRC_ADCValueUntersuchung_ADCDelay3.xlsx
+++ b/PhasenMethode/Messungen+Auswertung/Messungen/1312_HO_Amplitudenuntersuchung/05_InterleavingCodeRC_ADCValueUntersuchung_ADCDelay3.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i40014121\Desktop\Bachelorarbeit_Code\PhasenMethode\Messungen+Auswertung\Messungen\HO_1312_Amplitudenuntersuchung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i40014121\Desktop\Bachelorarbeit_Code\PhasenMethode\Messungen+Auswertung\Messungen\1312_HO_Amplitudenuntersuchung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0DD19827-973C-46A7-909B-40ECD408CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6F1CDB-2304-4D9A-96CE-85B2A7301F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05_InterleavingCodeRC_ADCValueU" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -932,7 +945,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2693,11 +2706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1658"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I34"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,7 +3136,7 @@
         <v>3</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:H25" si="8">H16+1</f>
+        <f t="shared" ref="H17" si="8">H16+1</f>
         <v>8</v>
       </c>
       <c r="I17" s="1" cm="1">
@@ -3151,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H16:H18" si="9">H16+1</f>
+        <f t="shared" ref="H18" si="9">H16+1</f>
         <v>8</v>
       </c>
       <c r="I18" s="1" cm="1">
@@ -3179,7 +3192,7 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H25" si="10">H18+1</f>
+        <f t="shared" ref="H19" si="10">H18+1</f>
         <v>9</v>
       </c>
       <c r="I19" s="1" cm="1">
@@ -3235,7 +3248,7 @@
         <v>3</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H25" si="12">H20+1</f>
+        <f t="shared" ref="H21" si="12">H20+1</f>
         <v>10</v>
       </c>
       <c r="I21" s="1" cm="1">
@@ -3291,7 +3304,7 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H25" si="14">H22+1</f>
+        <f t="shared" ref="H23" si="14">H22+1</f>
         <v>11</v>
       </c>
       <c r="I23" s="1" cm="1">
@@ -3403,7 +3416,7 @@
         <v>4</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H90" si="18">H26+1</f>
+        <f t="shared" ref="H27" si="18">H26+1</f>
         <v>13</v>
       </c>
       <c r="I27" s="1" cm="1">
@@ -3459,7 +3472,7 @@
         <v>4</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:H92" si="20">H28+1</f>
+        <f t="shared" ref="H29" si="20">H28+1</f>
         <v>14</v>
       </c>
       <c r="I29" s="1" cm="1">
@@ -3515,7 +3528,7 @@
         <v>4</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H94" si="22">H30+1</f>
+        <f t="shared" ref="H31" si="22">H30+1</f>
         <v>15</v>
       </c>
       <c r="I31" s="1" cm="1">
@@ -3571,7 +3584,7 @@
         <v>4</v>
       </c>
       <c r="H33">
-        <f t="shared" ref="H33:H96" si="24">H32+1</f>
+        <f t="shared" ref="H33" si="24">H32+1</f>
         <v>16</v>
       </c>
       <c r="I33" s="1" cm="1">
@@ -3627,7 +3640,7 @@
         <v>5</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H98" si="26">H34+1</f>
+        <f t="shared" ref="H35" si="26">H34+1</f>
         <v>17</v>
       </c>
       <c r="I35" s="1" cm="1">
@@ -3683,7 +3696,7 @@
         <v>5</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:H100" si="28">H36+1</f>
+        <f t="shared" ref="H37" si="28">H36+1</f>
         <v>18</v>
       </c>
       <c r="I37" s="1" cm="1">
@@ -3739,7 +3752,7 @@
         <v>5</v>
       </c>
       <c r="H39">
-        <f t="shared" ref="H39:H102" si="30">H38+1</f>
+        <f t="shared" ref="H39" si="30">H38+1</f>
         <v>19</v>
       </c>
       <c r="I39" s="1" cm="1">
@@ -3795,7 +3808,7 @@
         <v>5</v>
       </c>
       <c r="H41">
-        <f t="shared" ref="H41:H104" si="32">H40+1</f>
+        <f t="shared" ref="H41" si="32">H40+1</f>
         <v>20</v>
       </c>
       <c r="I41" s="1" cm="1">
@@ -3851,7 +3864,7 @@
         <v>6</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:H106" si="34">H42+1</f>
+        <f t="shared" ref="H43" si="34">H42+1</f>
         <v>21</v>
       </c>
       <c r="I43" s="1" cm="1">
@@ -3907,7 +3920,7 @@
         <v>6</v>
       </c>
       <c r="H45">
-        <f t="shared" ref="H45:H108" si="36">H44+1</f>
+        <f t="shared" ref="H45" si="36">H44+1</f>
         <v>22</v>
       </c>
       <c r="I45" s="1" cm="1">
@@ -3963,7 +3976,7 @@
         <v>6</v>
       </c>
       <c r="H47">
-        <f t="shared" ref="H47:H110" si="38">H46+1</f>
+        <f t="shared" ref="H47" si="38">H46+1</f>
         <v>23</v>
       </c>
       <c r="I47" s="1" cm="1">
@@ -4019,7 +4032,7 @@
         <v>6</v>
       </c>
       <c r="H49">
-        <f t="shared" ref="H49:H112" si="40">H48+1</f>
+        <f t="shared" ref="H49" si="40">H48+1</f>
         <v>24</v>
       </c>
       <c r="I49" s="1" cm="1">
@@ -4075,7 +4088,7 @@
         <v>6</v>
       </c>
       <c r="H51">
-        <f t="shared" ref="H51:H114" si="42">H50+1</f>
+        <f t="shared" ref="H51" si="42">H50+1</f>
         <v>25</v>
       </c>
       <c r="I51" s="1" cm="1">
@@ -4131,7 +4144,7 @@
         <v>7</v>
       </c>
       <c r="H53">
-        <f t="shared" ref="H53:H116" si="44">H52+1</f>
+        <f t="shared" ref="H53" si="44">H52+1</f>
         <v>26</v>
       </c>
       <c r="I53" s="1" cm="1">
@@ -4187,7 +4200,7 @@
         <v>7</v>
       </c>
       <c r="H55">
-        <f t="shared" ref="H55:H117" si="46">H54+1</f>
+        <f t="shared" ref="H55" si="46">H54+1</f>
         <v>27</v>
       </c>
       <c r="I55" s="1" cm="1">
@@ -4243,7 +4256,7 @@
         <v>7</v>
       </c>
       <c r="H57">
-        <f t="shared" ref="H57:H117" si="48">H56+1</f>
+        <f t="shared" ref="H57" si="48">H56+1</f>
         <v>28</v>
       </c>
       <c r="I57" s="1" cm="1">
@@ -4299,7 +4312,7 @@
         <v>7</v>
       </c>
       <c r="H59">
-        <f t="shared" ref="H59:H117" si="50">H58+1</f>
+        <f t="shared" ref="H59" si="50">H58+1</f>
         <v>29</v>
       </c>
       <c r="I59" s="1" cm="1">
@@ -4355,7 +4368,7 @@
         <v>8</v>
       </c>
       <c r="H61">
-        <f t="shared" ref="H61:H117" si="52">H60+1</f>
+        <f t="shared" ref="H61" si="52">H60+1</f>
         <v>30</v>
       </c>
       <c r="I61" s="1" cm="1">
@@ -4411,7 +4424,7 @@
         <v>8</v>
       </c>
       <c r="H63">
-        <f t="shared" ref="H63:H117" si="54">H62+1</f>
+        <f t="shared" ref="H63" si="54">H62+1</f>
         <v>31</v>
       </c>
       <c r="I63" s="1" cm="1">
@@ -4467,7 +4480,7 @@
         <v>8</v>
       </c>
       <c r="H65">
-        <f t="shared" ref="H65:H117" si="56">H64+1</f>
+        <f t="shared" ref="H65" si="56">H64+1</f>
         <v>32</v>
       </c>
       <c r="I65" s="1" cm="1">
@@ -4523,7 +4536,7 @@
         <v>8</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H117" si="58">H66+1</f>
+        <f t="shared" ref="H67" si="58">H66+1</f>
         <v>33</v>
       </c>
       <c r="I67" s="1" cm="1">
@@ -4579,7 +4592,7 @@
         <v>8</v>
       </c>
       <c r="H69">
-        <f t="shared" ref="H69:H117" si="60">H68+1</f>
+        <f t="shared" ref="H69" si="60">H68+1</f>
         <v>34</v>
       </c>
       <c r="I69" s="1" cm="1">
@@ -4635,7 +4648,7 @@
         <v>9</v>
       </c>
       <c r="H71">
-        <f t="shared" ref="H71:H117" si="62">H70+1</f>
+        <f t="shared" ref="H71" si="62">H70+1</f>
         <v>35</v>
       </c>
       <c r="I71" s="1" cm="1">
@@ -4691,7 +4704,7 @@
         <v>9</v>
       </c>
       <c r="H73">
-        <f t="shared" ref="H73:H117" si="64">H72+1</f>
+        <f t="shared" ref="H73" si="64">H72+1</f>
         <v>36</v>
       </c>
       <c r="I73" s="1" cm="1">
@@ -4747,7 +4760,7 @@
         <v>9</v>
       </c>
       <c r="H75">
-        <f t="shared" ref="H75:H117" si="66">H74+1</f>
+        <f t="shared" ref="H75" si="66">H74+1</f>
         <v>37</v>
       </c>
       <c r="I75" s="1" cm="1">
@@ -4803,7 +4816,7 @@
         <v>9</v>
       </c>
       <c r="H77">
-        <f t="shared" ref="H77:H117" si="68">H76+1</f>
+        <f t="shared" ref="H77" si="68">H76+1</f>
         <v>38</v>
       </c>
       <c r="I77" s="1" cm="1">
@@ -4859,7 +4872,7 @@
         <v>10</v>
       </c>
       <c r="H79">
-        <f t="shared" ref="H79:H117" si="70">H78+1</f>
+        <f t="shared" ref="H79" si="70">H78+1</f>
         <v>39</v>
       </c>
       <c r="I79" s="1" cm="1">
@@ -4915,7 +4928,7 @@
         <v>10</v>
       </c>
       <c r="H81">
-        <f t="shared" ref="H81:H117" si="72">H80+1</f>
+        <f t="shared" ref="H81" si="72">H80+1</f>
         <v>40</v>
       </c>
       <c r="I81" s="1" cm="1">
@@ -4971,7 +4984,7 @@
         <v>10</v>
       </c>
       <c r="H83">
-        <f t="shared" ref="H83:H117" si="74">H82+1</f>
+        <f t="shared" ref="H83" si="74">H82+1</f>
         <v>41</v>
       </c>
       <c r="I83" s="1" cm="1">
@@ -5027,7 +5040,7 @@
         <v>10</v>
       </c>
       <c r="H85">
-        <f t="shared" ref="H85:H117" si="76">H84+1</f>
+        <f t="shared" ref="H85" si="76">H84+1</f>
         <v>42</v>
       </c>
       <c r="I85" s="1" cm="1">
@@ -5083,7 +5096,7 @@
         <v>10</v>
       </c>
       <c r="H87">
-        <f t="shared" ref="H87:H117" si="78">H86+1</f>
+        <f t="shared" ref="H87" si="78">H86+1</f>
         <v>43</v>
       </c>
       <c r="I87" s="1" cm="1">
@@ -5139,7 +5152,7 @@
         <v>11</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89:H117" si="80">H88+1</f>
+        <f t="shared" ref="H89" si="80">H88+1</f>
         <v>44</v>
       </c>
       <c r="I89" s="1" cm="1">
@@ -5195,7 +5208,7 @@
         <v>11</v>
       </c>
       <c r="H91">
-        <f t="shared" ref="H91:H117" si="82">H90+1</f>
+        <f t="shared" ref="H91" si="82">H90+1</f>
         <v>45</v>
       </c>
       <c r="I91" s="1" cm="1">
@@ -5251,7 +5264,7 @@
         <v>11</v>
       </c>
       <c r="H93">
-        <f t="shared" ref="H93:H117" si="84">H92+1</f>
+        <f t="shared" ref="H93" si="84">H92+1</f>
         <v>46</v>
       </c>
       <c r="I93" s="1" cm="1">
@@ -5307,7 +5320,7 @@
         <v>11</v>
       </c>
       <c r="H95">
-        <f t="shared" ref="H95:H117" si="86">H94+1</f>
+        <f t="shared" ref="H95" si="86">H94+1</f>
         <v>47</v>
       </c>
       <c r="I95" s="1" cm="1">
@@ -5363,7 +5376,7 @@
         <v>12</v>
       </c>
       <c r="H97">
-        <f t="shared" ref="H97:H117" si="88">H96+1</f>
+        <f t="shared" ref="H97" si="88">H96+1</f>
         <v>48</v>
       </c>
       <c r="I97" s="1" cm="1">
@@ -5419,7 +5432,7 @@
         <v>12</v>
       </c>
       <c r="H99">
-        <f t="shared" ref="H99:H117" si="90">H98+1</f>
+        <f t="shared" ref="H99" si="90">H98+1</f>
         <v>49</v>
       </c>
       <c r="I99" s="1" cm="1">
@@ -5475,7 +5488,7 @@
         <v>12</v>
       </c>
       <c r="H101">
-        <f t="shared" ref="H101:H117" si="92">H100+1</f>
+        <f t="shared" ref="H101" si="92">H100+1</f>
         <v>50</v>
       </c>
       <c r="I101" s="1" cm="1">
@@ -5531,7 +5544,7 @@
         <v>12</v>
       </c>
       <c r="H103">
-        <f t="shared" ref="H103:H117" si="94">H102+1</f>
+        <f t="shared" ref="H103" si="94">H102+1</f>
         <v>51</v>
       </c>
       <c r="I103" s="1" cm="1">
@@ -5587,7 +5600,7 @@
         <v>12</v>
       </c>
       <c r="H105">
-        <f t="shared" ref="H105:H117" si="96">H104+1</f>
+        <f t="shared" ref="H105" si="96">H104+1</f>
         <v>52</v>
       </c>
       <c r="I105" s="1" cm="1">
@@ -5643,7 +5656,7 @@
         <v>13</v>
       </c>
       <c r="H107">
-        <f t="shared" ref="H107:H117" si="98">H106+1</f>
+        <f t="shared" ref="H107" si="98">H106+1</f>
         <v>53</v>
       </c>
       <c r="I107" s="1" cm="1">
@@ -5699,7 +5712,7 @@
         <v>13</v>
       </c>
       <c r="H109">
-        <f t="shared" ref="H109:H117" si="100">H108+1</f>
+        <f t="shared" ref="H109" si="100">H108+1</f>
         <v>54</v>
       </c>
       <c r="I109" s="1" cm="1">
@@ -5755,7 +5768,7 @@
         <v>13</v>
       </c>
       <c r="H111">
-        <f t="shared" ref="H111:H117" si="102">H110+1</f>
+        <f t="shared" ref="H111" si="102">H110+1</f>
         <v>55</v>
       </c>
       <c r="I111" s="1" cm="1">
@@ -5811,7 +5824,7 @@
         <v>13</v>
       </c>
       <c r="H113">
-        <f t="shared" ref="H113:H117" si="104">H112+1</f>
+        <f t="shared" ref="H113" si="104">H112+1</f>
         <v>56</v>
       </c>
       <c r="I113" s="1" cm="1">
@@ -5867,7 +5880,7 @@
         <v>14</v>
       </c>
       <c r="H115">
-        <f t="shared" ref="H115:H117" si="106">H114+1</f>
+        <f t="shared" ref="H115" si="106">H114+1</f>
         <v>57</v>
       </c>
       <c r="I115" s="1" cm="1">

</xml_diff>